<commit_message>
added the code for the pages Do pre-market engagement and Name your project
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/UI_TestData.xlsx
+++ b/src/test/resources/TestData/UI_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\571154\git\ccs-scale-cat-test-Master-29042022\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA1C3DB-9F52-4ADF-A793-98ED08386395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65600D96-5B5B-4ECB-9E8B-193773FC4948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{6F42FF04-6404-4D56-9108-23BBEBD1C648}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>TDID</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>1. See available suppliers!OPTIONAL!See available suppliers!2. Do pre-market engagement!OPTIONAL!Start pre-market engagement!3. Write and publish your requirements!TODO!Write and publish your requirements!4. Do evaluation!CANNOT START YET!5. Award the contract!CANNOT START YET!6. Publish your contract!OPTIONAL</t>
+  </si>
+  <si>
+    <t>DoPreMarketEngagementPageContentButtonStatus</t>
+  </si>
+  <si>
+    <t>Do pre-market engagement</t>
+  </si>
+  <si>
+    <t>1. Project and colleagues!Name your project!OPTIONAL!Change who is going to lead the procurement!OPTIONAL!Add colleagues to your project!OPTIONAL!2. Build your RfI!Build your RfI!TO DO!3. Review and publish your RfI!Upload documents!CANNOT START YET!See the suppliers who will receive your RfI!CANNOT START YET!Your RfI timeline!CANNOT START YET!Review and publish your RfI!CANNOT START YET</t>
+  </si>
+  <si>
+    <t>DoPreMarketEngagement_PageTitle</t>
   </si>
 </sst>
 </file>
@@ -661,10 +673,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA8D49A-BB20-4C74-9F3C-A1F46BC5FE7B}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -680,10 +692,12 @@
     <col min="10" max="10" width="17.90625" style="1" customWidth="1"/>
     <col min="11" max="11" width="18.7265625" style="1" customWidth="1"/>
     <col min="12" max="12" width="30.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="1"/>
+    <col min="13" max="13" width="30.453125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="44.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,8 +734,14 @@
       <c r="L1" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="174" x14ac:dyDescent="0.35">
+      <c r="M1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="174" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -758,8 +778,14 @@
       <c r="L2" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="174" x14ac:dyDescent="0.35">
+      <c r="M2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -795,6 +821,12 @@
       </c>
       <c r="L3" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the excel read method and added the code for 1FC journey
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/UI_TestData.xlsx
+++ b/src/test/resources/TestData/UI_TestData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\571154\git\ccs-scale-cat-test-Master-29042022\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65600D96-5B5B-4ECB-9E8B-193773FC4948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0CD9DE-5600-40F6-B7DE-73A2699F5439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{6F42FF04-6404-4D56-9108-23BBEBD1C648}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{6F42FF04-6404-4D56-9108-23BBEBD1C648}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateProject" sheetId="1" r:id="rId1"/>
     <sheet name="UpdateProject" sheetId="2" r:id="rId2"/>
     <sheet name="OneFCFlowTestData" sheetId="3" r:id="rId3"/>
+    <sheet name="OneFCFlowTestDataSanity" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
   <si>
     <t>TDID</t>
   </si>
@@ -166,6 +167,63 @@
   </si>
   <si>
     <t>DoPreMarketEngagement_PageTitle</t>
+  </si>
+  <si>
+    <t>data5</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>LoginPage</t>
+  </si>
+  <si>
+    <t>Sign in to the Public Procurement Gateway</t>
+  </si>
+  <si>
+    <t>Choose how to find a supplier</t>
+  </si>
+  <si>
+    <t>Write and publish your requirements</t>
+  </si>
+  <si>
+    <t>ChooseAgreement_Lot</t>
+  </si>
+  <si>
+    <t>S1_Title</t>
+  </si>
+  <si>
+    <t>S2_Radiobutton</t>
+  </si>
+  <si>
+    <t>S3_Title</t>
+  </si>
+  <si>
+    <t>1FC</t>
+  </si>
+  <si>
+    <t>Login_Title</t>
+  </si>
+  <si>
+    <t>Dashboard_Title</t>
+  </si>
+  <si>
+    <t>ChooseAgreement_Title</t>
+  </si>
+  <si>
+    <t>TDID1</t>
+  </si>
+  <si>
+    <t>UserID1</t>
+  </si>
+  <si>
+    <t>3. Write and publish your requirements</t>
+  </si>
+  <si>
+    <t>S1_Section</t>
+  </si>
+  <si>
+    <t>S2_Title</t>
   </si>
 </sst>
 </file>
@@ -675,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA8D49A-BB20-4C74-9F3C-A1F46BC5FE7B}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -746,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>21</v>
@@ -833,4 +891,177 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B7AC334-5A76-435C-B75A-0707E56AF15A}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="36.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7265625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="30.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.453125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="44.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Have added multiple java classes for 1FC
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/UI_TestData.xlsx
+++ b/src/test/resources/TestData/UI_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\571154\git\ccs-scale-cat-test-Master-29042022\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0CD9DE-5600-40F6-B7DE-73A2699F5439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CBBE9D-FF48-4E2E-83A4-A38C0DAB46AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{6F42FF04-6404-4D56-9108-23BBEBD1C648}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="141">
   <si>
     <t>TDID</t>
   </si>
@@ -224,6 +224,243 @@
   </si>
   <si>
     <t>S2_Title</t>
+  </si>
+  <si>
+    <t>2. Upload  pricing schedules and other documents</t>
+  </si>
+  <si>
+    <t>S4_Title</t>
+  </si>
+  <si>
+    <t>S5_Title</t>
+  </si>
+  <si>
+    <t>Upload your pricing schedule</t>
+  </si>
+  <si>
+    <t>S5_DocPath</t>
+  </si>
+  <si>
+    <t>C:\Users\571154\git\ccs-scale-cat-test-Master-29042022\src\test\resources\TestData\CSV.csv</t>
+  </si>
+  <si>
+    <t>2. Upload pricing schedules and other documents</t>
+  </si>
+  <si>
+    <t>Upload your terms and conditions and other documents</t>
+  </si>
+  <si>
+    <t>S6_DocPath</t>
+  </si>
+  <si>
+    <t>C:\Users\571154\git\ccs-scale-cat-test-Master-29042022\src\test\resources\TestData\DOC.doc</t>
+  </si>
+  <si>
+    <t>S6_Title</t>
+  </si>
+  <si>
+    <t>Confirm if you need a contracted out service or supply of resource</t>
+  </si>
+  <si>
+    <t>S7_Title</t>
+  </si>
+  <si>
+    <t>S7_Radiobutton</t>
+  </si>
+  <si>
+    <t>I need a contracted out service</t>
+  </si>
+  <si>
+    <t>S8_Title</t>
+  </si>
+  <si>
+    <t>About adding context and requirements</t>
+  </si>
+  <si>
+    <t>S9_Title</t>
+  </si>
+  <si>
+    <t>Terms and acronyms (Optional)</t>
+  </si>
+  <si>
+    <t>S10_Title</t>
+  </si>
+  <si>
+    <t>Add background to your procurement</t>
+  </si>
+  <si>
+    <t>S11_Title</t>
+  </si>
+  <si>
+    <t>S11_keyBackground</t>
+  </si>
+  <si>
+    <t>S11_SocialEcoEnvBenefits</t>
+  </si>
+  <si>
+    <t>TXT1-Write your key background information here</t>
+  </si>
+  <si>
+    <t>TXT2-Social value, economic and environmental benefits</t>
+  </si>
+  <si>
+    <t>The business problem you need to solve</t>
+  </si>
+  <si>
+    <t>S12_Title</t>
+  </si>
+  <si>
+    <t>The people who will use your product or service (Optional)</t>
+  </si>
+  <si>
+    <t>S13_Title</t>
+  </si>
+  <si>
+    <t>S14_Title</t>
+  </si>
+  <si>
+    <t>Work done so far (optional)</t>
+  </si>
+  <si>
+    <t>S15_Title</t>
+  </si>
+  <si>
+    <t>Which phase the project is in</t>
+  </si>
+  <si>
+    <t>S15_Radiobutton</t>
+  </si>
+  <si>
+    <t>Discovery</t>
+  </si>
+  <si>
+    <t>Which phases of the project you need resource for</t>
+  </si>
+  <si>
+    <t>S16_Title</t>
+  </si>
+  <si>
+    <t>S16_CheckboxDiscovery</t>
+  </si>
+  <si>
+    <t>S16_CheckboxAlpha</t>
+  </si>
+  <si>
+    <t>S16_CheckboxBeta</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>S16_CheckboxLive</t>
+  </si>
+  <si>
+    <t>S16_CheckboxServiceDesign</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>How long the project will last</t>
+  </si>
+  <si>
+    <t>S17_ProjectToStartDate</t>
+  </si>
+  <si>
+    <t>S17_HowLongProjectWillRunOptnalDate</t>
+  </si>
+  <si>
+    <t>S17_ExtensionPeriodOptnalDate</t>
+  </si>
+  <si>
+    <t>2/4/10</t>
+  </si>
+  <si>
+    <t>S12_BusinessProblemTextBox</t>
+  </si>
+  <si>
+    <t>The business problem you need to solve-TXT-1</t>
+  </si>
+  <si>
+    <t>Add context and requirements</t>
+  </si>
+  <si>
+    <t>0/5/1</t>
+  </si>
+  <si>
+    <t>Choose if this is new, replacement or expanded product or service</t>
+  </si>
+  <si>
+    <t>S20_Radiobutton</t>
+  </si>
+  <si>
+    <t>New products or services</t>
+  </si>
+  <si>
+    <t>Not sure</t>
+  </si>
+  <si>
+    <t>Tell us if there is an existing supplier</t>
+  </si>
+  <si>
+    <t>S21_Radiobutton</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>S21_Radiobutton_Yes_data</t>
+  </si>
+  <si>
+    <t>NODATA</t>
+  </si>
+  <si>
+    <t>Incumbent supplier-TXT</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Management information and reporting requirements</t>
+  </si>
+  <si>
+    <t>S22_TextBox</t>
+  </si>
+  <si>
+    <t>TXT1-Management information and reporting requirements</t>
+  </si>
+  <si>
+    <t>AddYourServiceLevelsAndKPIs</t>
+  </si>
+  <si>
+    <t>S23_TextBoxKPIs</t>
+  </si>
+  <si>
+    <t>A|A|10~B|B|11~C|C|12</t>
+  </si>
+  <si>
+    <t>AddAnyPerformanceIncentives</t>
+  </si>
+  <si>
+    <t>S24_PerformanceIncentivesTextbox</t>
+  </si>
+  <si>
+    <t>S24_ExitStrategyTextbox</t>
+  </si>
+  <si>
+    <t>TXT1-AddAnyPerformanceIncentives</t>
+  </si>
+  <si>
+    <t>TXT2-AddAnyPerformanceIncentives</t>
+  </si>
+  <si>
+    <t>S25_TextBoxProjectRequirements</t>
+  </si>
+  <si>
+    <t>A|A|A~B|B|B~C|C|C</t>
+  </si>
+  <si>
+    <t>EnterYourProjectRequirements</t>
   </si>
 </sst>
 </file>
@@ -265,13 +502,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -895,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B7AC334-5A76-435C-B75A-0707E56AF15A}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:AU4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -913,14 +1153,35 @@
     <col min="9" max="9" width="33.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="39.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="43" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.453125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="44.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.7265625" style="1"/>
+    <col min="14" max="15" width="30.453125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="44.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="56.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="32.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="34.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="34.7265625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="50.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="36" width="43.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="34.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="28.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="56.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="31.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="51.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="31.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="27.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:47" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -954,8 +1215,116 @@
       <c r="K1" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -989,8 +1358,116 @@
       <c r="K2" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:47" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1024,8 +1501,116 @@
       <c r="K3" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="L3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:47" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1058,6 +1643,114 @@
       </c>
       <c r="K4" s="2" t="s">
         <v>48</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>